<commit_message>
Initial implementation of auto-ranging
</commit_message>
<xml_diff>
--- a/documents/msp430_adc_characterization.xlsx
+++ b/documents/msp430_adc_characterization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andyj\Desktop\msp430-resistance-sensor\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE630B33-F3F5-48B3-8C16-D1C5168CA7E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDE0254-E5EE-48B2-A194-831BE6063F3F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{93B6BA8D-8C69-4A83-9023-06E499B8342F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t xml:space="preserve">Voltage </t>
   </si>
@@ -52,6 +52,30 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>21 &lt; x &lt; 60</t>
+  </si>
+  <si>
+    <t>61 &lt; x &lt; 300</t>
+  </si>
+  <si>
+    <t>301 &lt; x &lt; 600</t>
+  </si>
+  <si>
+    <t>601 &lt; x &lt; 6000</t>
+  </si>
+  <si>
+    <t>6001 &lt; x &lt; 60000</t>
+  </si>
+  <si>
+    <t>60001 &lt; x  &lt; 300000</t>
+  </si>
+  <si>
+    <t>1 &lt; x &lt; 20</t>
+  </si>
+  <si>
+    <t>3000001 &lt; x &lt; 1120000</t>
   </si>
 </sst>
 </file>
@@ -91,10 +115,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2553,10 +2577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F1DC89-E7A0-4EDD-B447-C3BFE65C24B2}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2564,19 +2588,19 @@
     <col min="1" max="1" width="14.21875" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2844,7 +2868,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>33</v>
       </c>
       <c r="B23">
@@ -2857,94 +2881,233 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>100</v>
       </c>
       <c r="B24">
-        <f xml:space="preserve"> (0.1*A24)/(3.3-0.1)</f>
+        <f t="shared" ref="B24:B30" si="0" xml:space="preserve"> (0.1*A24)/(3.3-0.1)</f>
         <v>3.1250000000000004</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:C30" si="0">(1.65*A24)/(3.3-1.65)</f>
+        <f t="shared" ref="C24:C30" si="1">(1.65*A24)/(3.3-1.65)</f>
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>470</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B24:B30" si="1" xml:space="preserve"> (0.1*A25)/(3.3-0.1)</f>
+        <f t="shared" si="0"/>
         <v>14.687500000000002</v>
       </c>
       <c r="C25">
+        <f t="shared" si="1"/>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B26">
         <f t="shared" si="0"/>
+        <v>31.250000000000004</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>312.5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>3125.0000000000005</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>560000</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>17500</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>560000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>1120000</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>35000</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>1120000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f xml:space="preserve"> (0.3*A34)/(3.3-0.3)</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="C34">
+        <f>(1.3*A34)/(3.3-1.3)</f>
+        <v>21.450000000000003</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>100</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ref="B35:B41" si="2" xml:space="preserve"> (0.3*A35)/(3.3-0.3)</f>
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C41" si="3">(1.3*A35)/(3.3-1.3)</f>
+        <v>65.000000000000014</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>470</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="B36">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="3"/>
+        <v>305.50000000000006</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>1000</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="1"/>
-        <v>31.250000000000004</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
+      <c r="B37">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="3"/>
+        <v>650.00000000000011</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="C38">
+        <f t="shared" si="3"/>
+        <v>6500.0000000000009</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="1"/>
-        <v>312.5</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
-        <v>100000</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="1"/>
-        <v>3125.0000000000005</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="C39">
+        <f>(1.3*A39)/(3.3-1.3)</f>
+        <v>65000.000000000007</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>560000</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="1"/>
-        <v>17500</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>560000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="B40">
+        <f t="shared" si="2"/>
+        <v>56000</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>364000.00000000006</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
         <v>1120000</v>
       </c>
-      <c r="B30">
-        <f t="shared" si="1"/>
-        <v>35000</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>1120000</v>
+      <c r="B41">
+        <f t="shared" si="2"/>
+        <v>112000</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>728000.00000000012</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement auto-ranging functionality (#9)
* Initial implementation of auto-ranging

* Add linker command script
</commit_message>
<xml_diff>
--- a/documents/msp430_adc_characterization.xlsx
+++ b/documents/msp430_adc_characterization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andyj\Desktop\msp430-resistance-sensor\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE630B33-F3F5-48B3-8C16-D1C5168CA7E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDE0254-E5EE-48B2-A194-831BE6063F3F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{93B6BA8D-8C69-4A83-9023-06E499B8342F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t xml:space="preserve">Voltage </t>
   </si>
@@ -52,6 +52,30 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>21 &lt; x &lt; 60</t>
+  </si>
+  <si>
+    <t>61 &lt; x &lt; 300</t>
+  </si>
+  <si>
+    <t>301 &lt; x &lt; 600</t>
+  </si>
+  <si>
+    <t>601 &lt; x &lt; 6000</t>
+  </si>
+  <si>
+    <t>6001 &lt; x &lt; 60000</t>
+  </si>
+  <si>
+    <t>60001 &lt; x  &lt; 300000</t>
+  </si>
+  <si>
+    <t>1 &lt; x &lt; 20</t>
+  </si>
+  <si>
+    <t>3000001 &lt; x &lt; 1120000</t>
   </si>
 </sst>
 </file>
@@ -91,10 +115,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2553,10 +2577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F1DC89-E7A0-4EDD-B447-C3BFE65C24B2}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2564,19 +2588,19 @@
     <col min="1" max="1" width="14.21875" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2844,7 +2868,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>33</v>
       </c>
       <c r="B23">
@@ -2857,94 +2881,233 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>100</v>
       </c>
       <c r="B24">
-        <f xml:space="preserve"> (0.1*A24)/(3.3-0.1)</f>
+        <f t="shared" ref="B24:B30" si="0" xml:space="preserve"> (0.1*A24)/(3.3-0.1)</f>
         <v>3.1250000000000004</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:C30" si="0">(1.65*A24)/(3.3-1.65)</f>
+        <f t="shared" ref="C24:C30" si="1">(1.65*A24)/(3.3-1.65)</f>
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>470</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B24:B30" si="1" xml:space="preserve"> (0.1*A25)/(3.3-0.1)</f>
+        <f t="shared" si="0"/>
         <v>14.687500000000002</v>
       </c>
       <c r="C25">
+        <f t="shared" si="1"/>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B26">
         <f t="shared" si="0"/>
+        <v>31.250000000000004</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>312.5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>3125.0000000000005</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>560000</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>17500</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>560000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>1120000</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>35000</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>1120000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f xml:space="preserve"> (0.3*A34)/(3.3-0.3)</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="C34">
+        <f>(1.3*A34)/(3.3-1.3)</f>
+        <v>21.450000000000003</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>100</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ref="B35:B41" si="2" xml:space="preserve"> (0.3*A35)/(3.3-0.3)</f>
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C41" si="3">(1.3*A35)/(3.3-1.3)</f>
+        <v>65.000000000000014</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>470</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="B36">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="3"/>
+        <v>305.50000000000006</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>1000</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="1"/>
-        <v>31.250000000000004</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
+      <c r="B37">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="3"/>
+        <v>650.00000000000011</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="C38">
+        <f t="shared" si="3"/>
+        <v>6500.0000000000009</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="1"/>
-        <v>312.5</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
-        <v>100000</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="1"/>
-        <v>3125.0000000000005</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="C39">
+        <f>(1.3*A39)/(3.3-1.3)</f>
+        <v>65000.000000000007</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>560000</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="1"/>
-        <v>17500</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>560000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="B40">
+        <f t="shared" si="2"/>
+        <v>56000</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>364000.00000000006</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
         <v>1120000</v>
       </c>
-      <c r="B30">
-        <f t="shared" si="1"/>
-        <v>35000</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>1120000</v>
+      <c r="B41">
+        <f t="shared" si="2"/>
+        <v>112000</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>728000.00000000012</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>